<commit_message>
fix program allocation error
</commit_message>
<xml_diff>
--- a/data/발표자_대쉬보드.xlsx
+++ b/data/발표자_대쉬보드.xlsx
@@ -26508,7 +26508,7 @@
   <dimension ref="A1:I993"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="16"/>
@@ -26761,7 +26761,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>122</v>

</xml_diff>